<commit_message>
Version 0.3 - 23.09.2024 - Change of substructure and code
</commit_message>
<xml_diff>
--- a/content/plastiq_input_information.xlsx
+++ b/content/plastiq_input_information.xlsx
@@ -9,6 +9,10 @@
     <sheet name="contact_data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="company_data" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="product_data" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="product_origin" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="product_fractions" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="product_quality" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="product_amount" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -2635,19 +2639,12 @@
           <t>2024-09-06 12:55:26</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr"/>
-      <c r="H62" t="inlineStr"/>
       <c r="I62" t="b">
         <v>0</v>
       </c>
       <c r="J62" t="b">
         <v>0</v>
       </c>
-      <c r="K62" t="inlineStr"/>
       <c r="L62" t="n">
         <v>44.933143</v>
       </c>
@@ -2669,7 +2666,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2817,6 +2814,670 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-09-16 09:30:27</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['Kunststoff – ABS', 'Kunststoff – ASA']</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>['ABS-Test', 'ASA-Test']</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>[90.0, 10.0]</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2024-09-16 12:10:56</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Post-Consumer (PC) – getrennte Sammlung</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>lokal als Bringsystem</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>12 15 15*</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2024-09-16 12:12:05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Post-Consumer (PC) – getrennte Sammlung</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>regional</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2024-09-16 12:15:18</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Post-Industrial (PI)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-09-16 12:19:11</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Post-Industrial (PI)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-09-16 12:19:24</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Post-Consumer (PC) – getrennte Sammlung</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>lokal als Bringsystem</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>15215</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-09-16 13:17:48</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Post-Industrial (PI)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-09-17 10:57:36</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Post-Industrial (PI)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2024-09-16 12:11:21</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>['Kunststoff – ABS', 'Kunststoff – ASA']</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>['', '']</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2024-09-16 13:17:45</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>['Kunststoff – ABS', 'Kunststoff – ABS']</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['', '']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2024-09-17 10:57:24</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>['Kunststoff – ABS', 'Kunststoff – ASA']</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['', '']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0]</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2024-09-16 14:03:27</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>blau</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>keine</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>['Antibeschlagmittel', 'Antibeschlagmittel']</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2024-09-16 14:03:50</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>blau</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>keine</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>['Antibeschlagmittel', 'Antibeschlagmittel']</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2024-09-16 14:08:01</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>blau</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>keine</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>['Antibeschlagmittel', 'Antibeschlagmittel', 'Antibeschlagmittel']</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0, 0.0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-09-17 11:19:33</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>100</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[['Antioxidant'], ['Gleitmittel']]</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-09-17 11:19:47</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>100</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[['Antioxidant', 'Biozide', 'Gleitmittel'], ['Gleitmittel', 'Antioxidant']]</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-09-19 11:22:09</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>100</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>[[], [], []]</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>[['Glimmer'], ['Ruß'], ['Glaskugeln', 'Glimmer', 'Glasfasern']]</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-09-19 11:26:11</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>100</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>[['Gleitmittel'], [], []]</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>[[], [], []]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2024-09-19 11:28:15</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>100</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>[[], [], []]</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>[[], [], []]</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2024-09-16 14:39:13</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Tag</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2024-09-16 14:40:18</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Tag</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Test
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2024-09-16 14:40:36</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Tag</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-09-16 14:41:38</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>20</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Woche</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>